<commit_message>
Fix formatting of mobile compare table.
Rename New Player Guide, to Player Guide.
</commit_message>
<xml_diff>
--- a/undyingkingdoms/static/metadata/modifiers.xlsx
+++ b/undyingkingdoms/static/metadata/modifiers.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,7 +410,7 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dwarven Made</t>
+          <t>Dwarven Steel</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -423,7 +423,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Dwarven Made: +15% Production Per Worker</t>
+          <t>Dwarven Steel: +15% Production Per Worker</t>
         </is>
       </c>
     </row>
@@ -535,11 +535,11 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Expendable: +10% Birth Rate</t>
+          <t>Expendable: +15% Birth Rate</t>
         </is>
       </c>
     </row>
@@ -564,11 +564,11 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Infighting: -2 Happiness</t>
+          <t>Infighting: -1 Happiness</t>
         </is>
       </c>
     </row>
@@ -578,43 +578,43 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Goblin</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Sneaky</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Infiltration Success Modifier</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Sneaky: +10% Infiltration Success</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Craftsman</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Production Per Worker Modifier</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Craftsman: +20% Production Per Worker</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -623,25 +623,25 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Merchant</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Silver Tongue</t>
+          <t>Artisan</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Income Modifier</t>
+          <t>Production Per Worker Modifier</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Silver Tongue: +15% Income</t>
+          <t>Artisan: +20% Production Per Worker</t>
         </is>
       </c>
     </row>
@@ -652,17 +652,17 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Rogue</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Army of Shadows</t>
+          <t>Craftsman</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Amount Of Thieves Modifier</t>
+          <t>Buildings Built Per Day Modifier</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -670,7 +670,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Army of Shadows: +2 Amount Of Thieves</t>
+          <t>Craftsman: +2 Buildings Built Per Day</t>
         </is>
       </c>
     </row>
@@ -681,25 +681,25 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Rogue</t>
+          <t>Merchant</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Master of Disguise</t>
+          <t>Silver Tongue</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Infiltration Success Modifier</t>
+          <t>Income Modifier</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Master of Disguise: +10% Infiltration Success</t>
+          <t>Silver Tongue: +15% Income</t>
         </is>
       </c>
     </row>
@@ -710,27 +710,415 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Rogue</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Army of Shadows</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Amount Of Thieves Modifier</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Army of Shadows: +2 Amount Of Thieves</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Rogue</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Master of Disguise</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Infiltration Success Modifier</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Master of Disguise: +15% Infiltration Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>Warlord</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Relentless</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Offensive Power Modifier</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F15" t="n">
         <v>0.15</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Relentless: +15% Offensive Power</t>
         </is>
       </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>